<commit_message>
sdg6 drop duplicate terms
</commit_message>
<xml_diff>
--- a/data/sdgs/SDG6.xlsx
+++ b/data/sdgs/SDG6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/glah/code/sustainability/keywords/data/sdgs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E97FC2A-67F0-D84C-BA7E-E72767137452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80418B53-AA46-B74F-AEFA-8E46D6293212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="920" windowWidth="28240" windowHeight="17240" xr2:uid="{F67271D4-E8A2-DA47-BD58-D76DCE882594}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="216">
   <si>
     <t>keyword_en</t>
   </si>
@@ -719,9 +719,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1096,7 +1095,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37E206DE-AB81-9F4A-B006-4986AE950285}">
   <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1153,2016 +1154,1986 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="1" t="s">
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" t="s">
         <v>28</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="1" t="s">
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="1" t="s">
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="1" t="s">
+      <c r="I5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" t="s">
         <v>32</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="L5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="1" t="s">
+      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" t="s">
         <v>36</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L6" s="1" t="s">
+      <c r="K6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="1" t="s">
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" s="1" t="s">
+      <c r="I7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" t="s">
         <v>36</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" t="s">
         <v>40</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="L7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="1" t="s">
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" s="1" t="s">
+      <c r="I8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" t="s">
         <v>36</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="K8" t="s">
         <v>44</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="L8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="1" t="s">
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" t="s">
         <v>35</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" t="s">
         <v>47</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" s="1" t="s">
+      <c r="I9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" t="s">
         <v>36</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="K9" t="s">
         <v>48</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="L9" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="1" t="s">
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" t="s">
         <v>35</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" t="s">
         <v>51</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" s="1" t="s">
+      <c r="I10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" t="s">
         <v>36</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="K10" t="s">
         <v>52</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="L10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="1" t="s">
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" t="s">
         <v>55</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J11" s="1" t="s">
+      <c r="I11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" t="s">
         <v>36</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="K11" t="s">
         <v>56</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="L11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" s="1" t="s">
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" t="s">
         <v>59</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J12" s="1" t="s">
+      <c r="H12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" t="s">
         <v>60</v>
       </c>
-      <c r="K12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L12" s="1" t="s">
+      <c r="K12" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="1" t="s">
+      <c r="E13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" t="s">
         <v>63</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J13" s="1" t="s">
+      <c r="H13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" t="s">
         <v>64</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L13" s="1" t="s">
+      <c r="K13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L13" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="1" t="s">
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="1" t="s">
+      <c r="E14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" t="s">
         <v>67</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J14" s="1" t="s">
+      <c r="H14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" t="s">
         <v>68</v>
       </c>
-      <c r="K14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L14" s="1" t="s">
+      <c r="K14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="1" t="s">
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
         <v>70</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="1" t="s">
+      <c r="E15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" t="s">
         <v>71</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J15" s="1" t="s">
+      <c r="H15" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" t="s">
         <v>72</v>
       </c>
-      <c r="K15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L15" s="1" t="s">
+      <c r="K15" t="s">
+        <v>14</v>
+      </c>
+      <c r="L15" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>73</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" s="1" t="s">
+      <c r="E16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" t="s">
         <v>75</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J16" s="1" t="s">
+      <c r="H16" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" t="s">
         <v>76</v>
       </c>
-      <c r="K16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L16" s="1" t="s">
+      <c r="K16" t="s">
+        <v>14</v>
+      </c>
+      <c r="L16" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>77</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="1" t="s">
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" t="s">
         <v>78</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="1" t="s">
+      <c r="E17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" t="s">
         <v>79</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J17" s="1" t="s">
+      <c r="H17" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17" t="s">
         <v>80</v>
       </c>
-      <c r="K17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L17" s="1" t="s">
+      <c r="K17" t="s">
+        <v>14</v>
+      </c>
+      <c r="L17" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>81</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L18" s="1" t="s">
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="K18" t="s">
+        <v>14</v>
+      </c>
+      <c r="L18" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>82</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="1" t="s">
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" t="s">
         <v>83</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="1" t="s">
+      <c r="E19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" t="s">
         <v>84</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J19" s="1" t="s">
+      <c r="H19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19" t="s">
         <v>85</v>
       </c>
-      <c r="K19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L19" s="1" t="s">
+      <c r="K19" t="s">
+        <v>14</v>
+      </c>
+      <c r="L19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>86</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" t="s">
         <v>87</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" s="1" t="s">
+      <c r="E20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" t="s">
         <v>88</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J20" s="1" t="s">
+      <c r="H20" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" t="s">
         <v>89</v>
       </c>
-      <c r="K20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L20" s="1" t="s">
+      <c r="K20" t="s">
+        <v>14</v>
+      </c>
+      <c r="L20" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" s="1" t="s">
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" t="s">
         <v>91</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J21" s="1" t="s">
+      <c r="H21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" t="s">
         <v>92</v>
       </c>
-      <c r="K21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L21" s="1" t="s">
+      <c r="K21" t="s">
+        <v>14</v>
+      </c>
+      <c r="L21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>93</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="1" t="s">
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" t="s">
         <v>94</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G22" s="1" t="s">
+      <c r="E22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" t="s">
         <v>95</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J22" s="1" t="s">
+      <c r="H22" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" t="s">
         <v>96</v>
       </c>
-      <c r="K22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L22" s="1" t="s">
+      <c r="K22" t="s">
+        <v>14</v>
+      </c>
+      <c r="L22" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>97</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="1" t="s">
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" t="s">
         <v>98</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G23" s="1" t="s">
+      <c r="E23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" t="s">
         <v>99</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J23" s="1" t="s">
+      <c r="H23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23" t="s">
+        <v>14</v>
+      </c>
+      <c r="J23" t="s">
         <v>100</v>
       </c>
-      <c r="K23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L23" s="1" t="s">
+      <c r="K23" t="s">
+        <v>14</v>
+      </c>
+      <c r="L23" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>101</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>102</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" s="1" t="s">
+      <c r="C24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" t="s">
         <v>103</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" t="s">
         <v>104</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G24" s="1" t="s">
+      <c r="F24" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" t="s">
         <v>105</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H24" t="s">
         <v>106</v>
       </c>
-      <c r="I24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J24" s="1" t="s">
+      <c r="I24" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24" t="s">
         <v>107</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="K24" t="s">
         <v>108</v>
       </c>
-      <c r="L24" s="1" t="s">
+      <c r="L24" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>101</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>109</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" s="1" t="s">
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" t="s">
         <v>103</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" t="s">
         <v>110</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G25" s="1" t="s">
+      <c r="F25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" t="s">
         <v>111</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="H25" t="s">
         <v>112</v>
       </c>
-      <c r="I25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J25" s="1" t="s">
+      <c r="I25" t="s">
+        <v>14</v>
+      </c>
+      <c r="J25" t="s">
         <v>107</v>
       </c>
-      <c r="K25" s="1" t="s">
+      <c r="K25" t="s">
         <v>113</v>
       </c>
-      <c r="L25" s="1" t="s">
+      <c r="L25" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>101</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>114</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" s="1" t="s">
+      <c r="C26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" t="s">
         <v>103</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E26" t="s">
         <v>115</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G26" s="1" t="s">
+      <c r="F26" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" t="s">
         <v>111</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="H26" t="s">
         <v>114</v>
       </c>
-      <c r="I26" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J26" s="1" t="s">
+      <c r="I26" t="s">
+        <v>14</v>
+      </c>
+      <c r="J26" t="s">
         <v>107</v>
       </c>
-      <c r="K26" s="1" t="s">
+      <c r="K26" t="s">
         <v>116</v>
       </c>
-      <c r="L26" s="1" t="s">
+      <c r="L26" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>101</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>117</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" s="1" t="s">
+      <c r="C27" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" t="s">
         <v>103</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" t="s">
         <v>118</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G27" s="1" t="s">
+      <c r="F27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" t="s">
         <v>105</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="H27" t="s">
         <v>119</v>
       </c>
-      <c r="I27" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J27" s="1" t="s">
+      <c r="I27" t="s">
+        <v>14</v>
+      </c>
+      <c r="J27" t="s">
         <v>107</v>
       </c>
-      <c r="K27" s="1" t="s">
+      <c r="K27" t="s">
         <v>120</v>
       </c>
-      <c r="L27" s="1" t="s">
+      <c r="L27" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>101</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>121</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="1" t="s">
+      <c r="C28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" t="s">
         <v>103</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" t="s">
         <v>122</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G28" s="1" t="s">
+      <c r="F28" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" t="s">
         <v>105</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="H28" t="s">
         <v>123</v>
       </c>
-      <c r="I28" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J28" s="1" t="s">
+      <c r="I28" t="s">
+        <v>14</v>
+      </c>
+      <c r="J28" t="s">
         <v>107</v>
       </c>
-      <c r="K28" s="1" t="s">
+      <c r="K28" t="s">
         <v>124</v>
       </c>
-      <c r="L28" s="1" t="s">
+      <c r="L28" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
+      <c r="A29" t="s">
         <v>101</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>125</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" s="1" t="s">
+      <c r="C29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" t="s">
         <v>103</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" t="s">
         <v>126</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G29" s="1" t="s">
+      <c r="F29" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" t="s">
         <v>105</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="H29" t="s">
         <v>127</v>
       </c>
-      <c r="I29" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J29" s="1" t="s">
+      <c r="I29" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" t="s">
         <v>107</v>
       </c>
-      <c r="K29" s="1" t="s">
+      <c r="K29" t="s">
         <v>128</v>
       </c>
-      <c r="L29" s="1" t="s">
+      <c r="L29" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
         <v>129</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
         <v>130</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D30" s="1" t="s">
+      <c r="C30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" t="s">
         <v>131</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" t="s">
         <v>132</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G30" s="1" t="s">
+      <c r="F30" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" t="s">
         <v>133</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="H30" t="s">
         <v>134</v>
       </c>
-      <c r="I30" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J30" s="1" t="s">
+      <c r="I30" t="s">
+        <v>14</v>
+      </c>
+      <c r="J30" t="s">
         <v>135</v>
       </c>
-      <c r="K30" s="1" t="s">
+      <c r="K30" t="s">
         <v>136</v>
       </c>
-      <c r="L30" s="1" t="s">
+      <c r="L30" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+      <c r="A31" t="s">
         <v>137</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" s="1" t="s">
+      <c r="B31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" t="s">
         <v>138</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G31" s="1" t="s">
+      <c r="E31" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" t="s">
         <v>139</v>
       </c>
-      <c r="H31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J31" s="1" t="s">
+      <c r="H31" t="s">
+        <v>14</v>
+      </c>
+      <c r="I31" t="s">
+        <v>14</v>
+      </c>
+      <c r="J31" t="s">
         <v>140</v>
       </c>
-      <c r="K31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L31" s="1" t="s">
+      <c r="K31" t="s">
+        <v>14</v>
+      </c>
+      <c r="L31" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+      <c r="A32" t="s">
         <v>141</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D32" s="1" t="s">
+      <c r="B32" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" t="s">
         <v>142</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G32" s="1" t="s">
+      <c r="E32" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" t="s">
         <v>143</v>
       </c>
-      <c r="H32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J32" s="1" t="s">
+      <c r="H32" t="s">
+        <v>14</v>
+      </c>
+      <c r="I32" t="s">
+        <v>14</v>
+      </c>
+      <c r="J32" t="s">
         <v>144</v>
       </c>
-      <c r="K32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L32" s="1" t="s">
+      <c r="K32" t="s">
+        <v>14</v>
+      </c>
+      <c r="L32" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+      <c r="A33" t="s">
         <v>145</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D33" s="1" t="s">
+      <c r="B33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" t="s">
         <v>146</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G33" s="1" t="s">
+      <c r="E33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33" t="s">
         <v>147</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J33" s="1" t="s">
+      <c r="H33" t="s">
+        <v>14</v>
+      </c>
+      <c r="I33" t="s">
+        <v>14</v>
+      </c>
+      <c r="J33" t="s">
         <v>148</v>
       </c>
-      <c r="K33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L33" s="1" t="s">
+      <c r="K33" t="s">
+        <v>14</v>
+      </c>
+      <c r="L33" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+      <c r="A34" t="s">
         <v>149</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34" s="1" t="s">
+      <c r="B34" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" t="s">
         <v>150</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G34" s="1" t="s">
+      <c r="E34" t="s">
+        <v>14</v>
+      </c>
+      <c r="F34" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" t="s">
         <v>151</v>
       </c>
-      <c r="H34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J34" s="1" t="s">
+      <c r="H34" t="s">
+        <v>14</v>
+      </c>
+      <c r="I34" t="s">
+        <v>14</v>
+      </c>
+      <c r="J34" t="s">
         <v>152</v>
       </c>
-      <c r="K34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L34" s="1" t="s">
+      <c r="K34" t="s">
+        <v>14</v>
+      </c>
+      <c r="L34" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+      <c r="A35" t="s">
         <v>153</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D35" s="1" t="s">
+      <c r="B35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" t="s">
         <v>154</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G35" s="1" t="s">
+      <c r="E35" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35" t="s">
         <v>155</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J35" s="1" t="s">
+      <c r="H35" t="s">
+        <v>14</v>
+      </c>
+      <c r="I35" t="s">
+        <v>14</v>
+      </c>
+      <c r="J35" t="s">
         <v>156</v>
       </c>
-      <c r="K35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L35" s="1" t="s">
+      <c r="K35" t="s">
+        <v>14</v>
+      </c>
+      <c r="L35" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>157</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D36" s="1" t="s">
+      <c r="B36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" t="s">
         <v>158</v>
       </c>
-      <c r="E36" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G36" s="1" t="s">
+      <c r="E36" t="s">
+        <v>14</v>
+      </c>
+      <c r="F36" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" t="s">
         <v>159</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J36" s="1" t="s">
+      <c r="H36" t="s">
+        <v>14</v>
+      </c>
+      <c r="I36" t="s">
+        <v>14</v>
+      </c>
+      <c r="J36" t="s">
         <v>160</v>
       </c>
-      <c r="K36" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L36" s="1" t="s">
+      <c r="K36" t="s">
+        <v>14</v>
+      </c>
+      <c r="L36" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+      <c r="A37" t="s">
         <v>161</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D37" s="1" t="s">
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" t="s">
         <v>162</v>
       </c>
-      <c r="E37" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G37" s="1" t="s">
+      <c r="E37" t="s">
+        <v>14</v>
+      </c>
+      <c r="F37" t="s">
+        <v>14</v>
+      </c>
+      <c r="G37" t="s">
         <v>163</v>
       </c>
-      <c r="H37" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J37" s="1" t="s">
+      <c r="H37" t="s">
+        <v>14</v>
+      </c>
+      <c r="I37" t="s">
+        <v>14</v>
+      </c>
+      <c r="J37" t="s">
         <v>164</v>
       </c>
-      <c r="K37" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L37" s="1" t="s">
+      <c r="K37" t="s">
+        <v>14</v>
+      </c>
+      <c r="L37" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+      <c r="A38" t="s">
         <v>53</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" t="s">
         <v>165</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D38" s="1" t="s">
+      <c r="C38" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" t="s">
         <v>54</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" t="s">
         <v>166</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G38" s="1" t="s">
+      <c r="F38" t="s">
+        <v>14</v>
+      </c>
+      <c r="G38" t="s">
         <v>55</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="H38" t="s">
         <v>167</v>
       </c>
-      <c r="I38" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J38" s="1" t="s">
+      <c r="I38" t="s">
+        <v>14</v>
+      </c>
+      <c r="J38" t="s">
         <v>56</v>
       </c>
-      <c r="K38" s="1" t="s">
+      <c r="K38" t="s">
         <v>168</v>
       </c>
-      <c r="L38" s="1" t="s">
+      <c r="L38" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+      <c r="A39" t="s">
         <v>82</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" t="s">
         <v>169</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D39" s="1" t="s">
+      <c r="C39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" t="s">
         <v>83</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" t="s">
         <v>170</v>
       </c>
-      <c r="F39" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G39" s="1" t="s">
+      <c r="F39" t="s">
+        <v>14</v>
+      </c>
+      <c r="G39" t="s">
         <v>84</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="H39" t="s">
         <v>171</v>
       </c>
-      <c r="I39" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J39" s="1" t="s">
+      <c r="I39" t="s">
+        <v>14</v>
+      </c>
+      <c r="J39" t="s">
         <v>85</v>
       </c>
-      <c r="K39" s="1" t="s">
+      <c r="K39" t="s">
         <v>172</v>
       </c>
-      <c r="L39" s="1" t="s">
+      <c r="L39" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+      <c r="A40" t="s">
         <v>82</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" t="s">
         <v>173</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D40" s="1" t="s">
+      <c r="C40" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" t="s">
         <v>174</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" t="s">
         <v>175</v>
       </c>
-      <c r="F40" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G40" s="1" t="s">
+      <c r="F40" t="s">
+        <v>14</v>
+      </c>
+      <c r="G40" t="s">
         <v>84</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="H40" t="s">
         <v>176</v>
       </c>
-      <c r="I40" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J40" s="1" t="s">
+      <c r="I40" t="s">
+        <v>14</v>
+      </c>
+      <c r="J40" t="s">
         <v>85</v>
       </c>
-      <c r="K40" s="1" t="s">
+      <c r="K40" t="s">
         <v>177</v>
       </c>
-      <c r="L40" s="1" t="s">
+      <c r="L40" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A41" s="1" t="s">
+      <c r="A41" t="s">
         <v>178</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" t="s">
         <v>101</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D41" s="1" t="s">
+      <c r="C41" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" t="s">
         <v>179</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E41" t="s">
         <v>103</v>
       </c>
-      <c r="F41" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G41" s="1" t="s">
+      <c r="F41" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" t="s">
         <v>180</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="H41" t="s">
         <v>111</v>
       </c>
-      <c r="I41" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J41" s="1" t="s">
+      <c r="I41" t="s">
+        <v>14</v>
+      </c>
+      <c r="J41" t="s">
         <v>181</v>
       </c>
-      <c r="K41" s="1" t="s">
+      <c r="K41" t="s">
         <v>107</v>
       </c>
-      <c r="L41" s="1" t="s">
+      <c r="L41" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+      <c r="A42" t="s">
         <v>101</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D42" s="1" t="s">
+      <c r="B42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" t="s">
         <v>103</v>
       </c>
-      <c r="E42" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G42" s="1" t="s">
+      <c r="E42" t="s">
+        <v>14</v>
+      </c>
+      <c r="F42" t="s">
+        <v>14</v>
+      </c>
+      <c r="G42" t="s">
         <v>111</v>
       </c>
-      <c r="H42" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J42" s="1" t="s">
+      <c r="H42" t="s">
+        <v>14</v>
+      </c>
+      <c r="I42" t="s">
+        <v>14</v>
+      </c>
+      <c r="J42" t="s">
         <v>107</v>
       </c>
-      <c r="K42" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L42" s="1" t="s">
+      <c r="K42" t="s">
+        <v>14</v>
+      </c>
+      <c r="L42" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A43" s="1" t="s">
+      <c r="A43" t="s">
         <v>149</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D43" s="1" t="s">
+      <c r="B43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" t="s">
         <v>150</v>
       </c>
-      <c r="E43" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G43" s="1" t="s">
+      <c r="E43" t="s">
+        <v>14</v>
+      </c>
+      <c r="F43" t="s">
+        <v>14</v>
+      </c>
+      <c r="G43" t="s">
         <v>151</v>
       </c>
-      <c r="H43" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J43" s="1" t="s">
+      <c r="H43" t="s">
+        <v>14</v>
+      </c>
+      <c r="I43" t="s">
+        <v>14</v>
+      </c>
+      <c r="J43" t="s">
         <v>152</v>
       </c>
-      <c r="K43" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L43" s="1" t="s">
+      <c r="K43" t="s">
+        <v>14</v>
+      </c>
+      <c r="L43" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
+      <c r="A44" t="s">
         <v>182</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G44" s="1" t="s">
+      <c r="B44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" t="s">
+        <v>14</v>
+      </c>
+      <c r="E44" t="s">
+        <v>14</v>
+      </c>
+      <c r="F44" t="s">
+        <v>14</v>
+      </c>
+      <c r="G44" t="s">
         <v>183</v>
       </c>
-      <c r="H44" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J44" s="1" t="s">
+      <c r="H44" t="s">
+        <v>14</v>
+      </c>
+      <c r="I44" t="s">
+        <v>14</v>
+      </c>
+      <c r="J44" t="s">
         <v>184</v>
       </c>
-      <c r="K44" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L44" s="1" t="s">
+      <c r="K44" t="s">
+        <v>14</v>
+      </c>
+      <c r="L44" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+      <c r="A45" t="s">
         <v>185</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" t="s">
         <v>130</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D45" s="1" t="s">
+      <c r="C45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45" t="s">
         <v>131</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E45" t="s">
         <v>132</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G45" s="1" t="s">
+      <c r="F45" t="s">
+        <v>14</v>
+      </c>
+      <c r="G45" t="s">
         <v>133</v>
       </c>
-      <c r="H45" s="1" t="s">
+      <c r="H45" t="s">
         <v>134</v>
       </c>
-      <c r="I45" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J45" s="1" t="s">
+      <c r="I45" t="s">
+        <v>14</v>
+      </c>
+      <c r="J45" t="s">
         <v>186</v>
       </c>
-      <c r="K45" s="1" t="s">
+      <c r="K45" t="s">
         <v>136</v>
       </c>
-      <c r="L45" s="1" t="s">
+      <c r="L45" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+      <c r="A46" t="s">
         <v>185</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" t="s">
         <v>129</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D46" s="1" t="s">
+      <c r="C46" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" t="s">
         <v>187</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E46" t="s">
         <v>188</v>
       </c>
-      <c r="F46" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G46" s="1" t="s">
+      <c r="F46" t="s">
+        <v>14</v>
+      </c>
+      <c r="G46" t="s">
         <v>189</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="H46" t="s">
         <v>133</v>
       </c>
-      <c r="I46" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J46" s="1" t="s">
+      <c r="I46" t="s">
+        <v>14</v>
+      </c>
+      <c r="J46" t="s">
         <v>135</v>
       </c>
-      <c r="K46" s="1" t="s">
+      <c r="K46" t="s">
         <v>186</v>
       </c>
-      <c r="L46" s="1" t="s">
+      <c r="L46" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
+      <c r="A47" t="s">
         <v>185</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" t="s">
         <v>130</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D47" s="1" t="s">
+      <c r="C47" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" t="s">
         <v>187</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E47" t="s">
         <v>132</v>
       </c>
-      <c r="F47" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G47" s="1" t="s">
+      <c r="F47" t="s">
+        <v>14</v>
+      </c>
+      <c r="G47" t="s">
         <v>189</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="H47" t="s">
         <v>134</v>
       </c>
-      <c r="I47" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J47" s="1" t="s">
+      <c r="I47" t="s">
+        <v>14</v>
+      </c>
+      <c r="J47" t="s">
         <v>135</v>
       </c>
-      <c r="K47" s="1" t="s">
+      <c r="K47" t="s">
         <v>136</v>
       </c>
-      <c r="L47" s="1" t="s">
+      <c r="L47" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
+      <c r="A48" t="s">
         <v>190</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D48" s="1" t="s">
+      <c r="B48" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48" t="s">
         <v>191</v>
       </c>
-      <c r="E48" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G48" s="1" t="s">
+      <c r="E48" t="s">
+        <v>14</v>
+      </c>
+      <c r="F48" t="s">
+        <v>14</v>
+      </c>
+      <c r="G48" t="s">
         <v>192</v>
       </c>
-      <c r="H48" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I48" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J48" s="1" t="s">
+      <c r="H48" t="s">
+        <v>14</v>
+      </c>
+      <c r="I48" t="s">
+        <v>14</v>
+      </c>
+      <c r="J48" t="s">
         <v>193</v>
       </c>
-      <c r="K48" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L48" s="1" t="s">
+      <c r="K48" t="s">
+        <v>14</v>
+      </c>
+      <c r="L48" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
+      <c r="A49" t="s">
         <v>194</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D49" s="1" t="s">
+      <c r="B49" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" t="s">
         <v>126</v>
       </c>
-      <c r="E49" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G49" s="1" t="s">
+      <c r="E49" t="s">
+        <v>14</v>
+      </c>
+      <c r="F49" t="s">
+        <v>14</v>
+      </c>
+      <c r="G49" t="s">
         <v>127</v>
       </c>
-      <c r="H49" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J49" s="1" t="s">
+      <c r="H49" t="s">
+        <v>14</v>
+      </c>
+      <c r="I49" t="s">
+        <v>14</v>
+      </c>
+      <c r="J49" t="s">
         <v>195</v>
       </c>
-      <c r="K49" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L49" s="1" t="s">
+      <c r="K49" t="s">
+        <v>14</v>
+      </c>
+      <c r="L49" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
+      <c r="A50" t="s">
         <v>196</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D50" s="1" t="s">
+      <c r="B50" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" t="s">
+        <v>14</v>
+      </c>
+      <c r="D50" t="s">
         <v>197</v>
       </c>
-      <c r="E50" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G50" s="1" t="s">
+      <c r="E50" t="s">
+        <v>14</v>
+      </c>
+      <c r="F50" t="s">
+        <v>14</v>
+      </c>
+      <c r="G50" t="s">
         <v>198</v>
       </c>
-      <c r="H50" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J50" s="1" t="s">
+      <c r="H50" t="s">
+        <v>14</v>
+      </c>
+      <c r="I50" t="s">
+        <v>14</v>
+      </c>
+      <c r="J50" t="s">
         <v>199</v>
       </c>
-      <c r="K50" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L50" s="1" t="s">
+      <c r="K50" t="s">
+        <v>14</v>
+      </c>
+      <c r="L50" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
+      <c r="A51" t="s">
         <v>200</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D51" s="1" t="s">
+      <c r="B51" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51" t="s">
+        <v>14</v>
+      </c>
+      <c r="D51" t="s">
         <v>201</v>
       </c>
-      <c r="E51" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G51" s="1" t="s">
+      <c r="E51" t="s">
+        <v>14</v>
+      </c>
+      <c r="F51" t="s">
+        <v>14</v>
+      </c>
+      <c r="G51" t="s">
         <v>202</v>
       </c>
-      <c r="H51" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J51" s="1" t="s">
+      <c r="H51" t="s">
+        <v>14</v>
+      </c>
+      <c r="I51" t="s">
+        <v>14</v>
+      </c>
+      <c r="J51" t="s">
         <v>203</v>
       </c>
-      <c r="K51" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L51" s="1" t="s">
+      <c r="K51" t="s">
+        <v>14</v>
+      </c>
+      <c r="L51" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
+      <c r="A52" t="s">
         <v>204</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D52" s="1" t="s">
+      <c r="B52" t="s">
+        <v>14</v>
+      </c>
+      <c r="C52" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" t="s">
         <v>205</v>
       </c>
-      <c r="E52" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G52" s="1" t="s">
+      <c r="E52" t="s">
+        <v>14</v>
+      </c>
+      <c r="F52" t="s">
+        <v>14</v>
+      </c>
+      <c r="G52" t="s">
         <v>206</v>
       </c>
-      <c r="H52" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J52" s="1" t="s">
+      <c r="H52" t="s">
+        <v>14</v>
+      </c>
+      <c r="I52" t="s">
+        <v>14</v>
+      </c>
+      <c r="J52" t="s">
         <v>207</v>
       </c>
-      <c r="K52" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L52" s="1" t="s">
+      <c r="K52" t="s">
+        <v>14</v>
+      </c>
+      <c r="L52" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
+      <c r="A53" t="s">
         <v>208</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D53" s="1" t="s">
+      <c r="B53" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" t="s">
+        <v>14</v>
+      </c>
+      <c r="D53" t="s">
         <v>209</v>
       </c>
-      <c r="E53" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G53" s="1" t="s">
+      <c r="E53" t="s">
+        <v>14</v>
+      </c>
+      <c r="F53" t="s">
+        <v>14</v>
+      </c>
+      <c r="G53" t="s">
         <v>210</v>
       </c>
-      <c r="H53" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J53" s="1" t="s">
+      <c r="H53" t="s">
+        <v>14</v>
+      </c>
+      <c r="I53" t="s">
+        <v>14</v>
+      </c>
+      <c r="J53" t="s">
         <v>211</v>
       </c>
-      <c r="K53" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L53" s="1" t="s">
+      <c r="K53" t="s">
+        <v>14</v>
+      </c>
+      <c r="L53" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
+      <c r="A54" t="s">
         <v>212</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D54" s="1" t="s">
+      <c r="B54" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54" t="s">
         <v>213</v>
       </c>
-      <c r="E54" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G54" s="1" t="s">
+      <c r="E54" t="s">
+        <v>14</v>
+      </c>
+      <c r="F54" t="s">
+        <v>14</v>
+      </c>
+      <c r="G54" t="s">
         <v>214</v>
       </c>
-      <c r="H54" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J54" s="1" t="s">
+      <c r="H54" t="s">
+        <v>14</v>
+      </c>
+      <c r="I54" t="s">
+        <v>14</v>
+      </c>
+      <c r="J54" t="s">
         <v>215</v>
       </c>
-      <c r="K54" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L54" s="1" t="s">
+      <c r="K54" t="s">
+        <v>14</v>
+      </c>
+      <c r="L54" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>